<commit_message>
modified excel files in static
</commit_message>
<xml_diff>
--- a/static/AS2.CTE.Relationships.xlsx
+++ b/static/AS2.CTE.Relationships.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\08187U744\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhyan/Documents/Tasks/HTTP_API_Server/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30833AAD-DC90-4D5D-8F88-650907B03543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C493E544-A191-CF41-B1ED-4E39CAC891EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25380" windowHeight="13660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,6 +395,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -759,12 +760,12 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -894,7 +895,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -956,7 +957,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>106</v>
       </c>

</xml_diff>